<commit_message>
updated excel data and headers
</commit_message>
<xml_diff>
--- a/Systems.xlsx
+++ b/Systems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagar.prasad/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilesh.heda\code\Sagar\rule-editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14ECF07F-FB6F-DD48-8BC9-DDA7C5861984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E481A7-C407-458E-BB89-4DC7BF3DF991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{28B2B8D7-8A39-8645-A9B0-54D055B01E4B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{28B2B8D7-8A39-8645-A9B0-54D055B01E4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="101">
   <si>
     <t>Platform Service</t>
   </si>
@@ -137,18 +137,6 @@
     <t>Analytics System</t>
   </si>
   <si>
-    <t>RRA</t>
-  </si>
-  <si>
-    <t>ClickHouse</t>
-  </si>
-  <si>
-    <t>Databricks</t>
-  </si>
-  <si>
-    <t>Tabelue</t>
-  </si>
-  <si>
     <t>ESB (Enterprise Service Bus)</t>
   </si>
   <si>
@@ -255,9 +243,6 @@
   </si>
   <si>
     <t xml:space="preserve">RRA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">over emails </t>
   </si>
   <si>
     <t xml:space="preserve">Excel </t>
@@ -338,6 +323,24 @@
   </si>
   <si>
     <t>Picking, Packing, QC, Returns, Receiving, Dispatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan vs Actual monitoring </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emails </t>
+  </si>
+  <si>
+    <t>SAP Financial</t>
+  </si>
+  <si>
+    <t>POSDTA, SAP financial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP/ Herald / ROMS </t>
+  </si>
+  <si>
+    <t>RRA, Clickhouse, Databricks, Tableu</t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -739,20 +738,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06262CDC-C76D-764A-8F54-3F814DB2115F}">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C54" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.19921875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -763,7 +762,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -771,7 +770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -782,7 +781,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -790,7 +789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -798,393 +797,388 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C12" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>95</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>75</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>89</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C46" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>63</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C53" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>34</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="2" t="s">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="B62" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B77" s="2" t="s">
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="B63" s="2" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>43</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>45</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B45:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>